<commit_message>
Remoção de erros e redimencionamento da home page
</commit_message>
<xml_diff>
--- a/cronograma.xlsx
+++ b/cronograma.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -30,6 +30,15 @@
   </si>
   <si>
     <t xml:space="preserve">ID da Turma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-03-31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-03-16</t>
   </si>
 </sst>
 </file>
@@ -308,6 +317,26 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>233</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>